<commit_message>
Updated pizzas spreadsheet - relaced vegan 'food' with food
</commit_message>
<xml_diff>
--- a/pizzas.xlsx
+++ b/pizzas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve.hughes\Desktop\Brighton alt.net\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\brighton-alt-net\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F11892-AA10-4066-B3CD-BC0628CF2024}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB32AF9-237B-450D-880C-DCC5D984F042}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{2B3E99AC-C6C9-47E9-9DBB-4BB115C8EBDC}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>quantity</t>
   </si>
@@ -38,27 +38,9 @@
     <t>pizza</t>
   </si>
   <si>
-    <t>Thom Yorke</t>
-  </si>
-  <si>
-    <t>Margherita</t>
-  </si>
-  <si>
-    <t>Johnno</t>
-  </si>
-  <si>
     <t>Jakub</t>
   </si>
   <si>
-    <t>Nadine GF</t>
-  </si>
-  <si>
-    <t>Woodsman</t>
-  </si>
-  <si>
-    <t>Funghi</t>
-  </si>
-  <si>
     <t>Vesuvius</t>
   </si>
   <si>
@@ -78,6 +60,27 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Funghi (v)</t>
+  </si>
+  <si>
+    <t>Gluten free (+£3)</t>
+  </si>
+  <si>
+    <t>Johnno (v)</t>
+  </si>
+  <si>
+    <t>Margherita (v)</t>
+  </si>
+  <si>
+    <t>Margherita GF (v)</t>
+  </si>
+  <si>
+    <t>Parma</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,6 +194,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,201 +511,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8616351-E355-4A61-A6CC-7579DB90D8AF}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D14"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7">
+        <f t="shared" ref="E2:E9" si="0">C2*D2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7">
-        <v>10</v>
-      </c>
-      <c r="D2" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="E3" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7">
         <v>1</v>
-      </c>
-      <c r="C3" s="7">
-        <v>7</v>
-      </c>
-      <c r="D3" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7">
-        <v>10</v>
       </c>
       <c r="D4" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="D5" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6">
+        <f>SUM(C2:C9)</f>
+        <v>11</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8">
+        <f>SUM(E2:E9)</f>
+        <v>116.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8">
+        <f>0.1*E11</f>
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="7">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>9.5</v>
-      </c>
-      <c r="D9" s="7">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="7">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7">
-        <v>11</v>
-      </c>
-      <c r="D10" s="7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6">
-        <f>SUM(B2:B10)</f>
-        <v>11</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8">
-        <f>SUM(D2:D10)</f>
-        <v>109.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8">
-        <f>0.1*D12</f>
-        <v>10.950000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4">
-        <f>0.9*D12</f>
-        <v>98.55</v>
+      <c r="B13" s="9"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4">
+        <f>0.9*E11</f>
+        <v>104.85000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pizzas spreadsheet - formatting
</commit_message>
<xml_diff>
--- a/pizzas.xlsx
+++ b/pizzas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\brighton-alt-net\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB32AF9-237B-450D-880C-DCC5D984F042}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81CBCE1-9D21-45E3-990D-E4EFA0C6EC5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{2B3E99AC-C6C9-47E9-9DBB-4BB115C8EBDC}"/>
   </bookViews>
@@ -125,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -134,10 +134,40 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -147,8 +177,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -158,7 +192,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -168,35 +204,161 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +676,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,195 +689,195 @@
     <col min="6" max="6" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11">
         <v>1</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="11">
         <v>8</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="16">
         <f t="shared" ref="E2:E9" si="0">C2*D2</f>
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="2">
         <v>11</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="2">
         <v>10</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="2">
         <v>12</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7">
+      <c r="B6" s="1"/>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="2">
         <v>10.5</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="18">
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="2">
         <v>11</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2">
         <v>2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="2">
         <v>10.5</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="18">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2">
         <v>3</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="2">
         <v>11</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="18">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1">
         <f>SUM(C2:C9)</f>
         <v>11</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8">
+      <c r="D11" s="3"/>
+      <c r="E11" s="20">
         <f>SUM(E2:E9)</f>
         <v>116.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="22">
         <f>0.1*E11</f>
         <v>11.65</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9">
         <f>0.9*E11</f>
         <v>104.85000000000001</v>
       </c>

</xml_diff>